<commit_message>
Ver 6.1.6.2 20241009 - Release to MOWong for UnisemIpoh, LYL/YZ for UnisemCD - Gitted - [BugFix] Remove IOState buzzer ignore, allow buzzer to function for alarm message. - YZ. - [BugFix] Corrected btn_HeadOfstTouchDotSet_Click to update TaskDisp. TeachNeedle_Completed. - MO Wong. - [Improve] Added debung info to MoveToOut and remove Thread.Sleep(5). Need monitor for conv not moving. -  YZ.
</commit_message>
<xml_diff>
--- a/Doc/UnisemCD A300 Item Tracking.xlsx
+++ b/Doc/UnisemCD A300 Item Tracking.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SW_KN_2403\GitHub - Source\NDispWin5-Unisem-x64\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0DDCD18-E0AA-4393-995F-5C690B084528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245135AE-7E35-4D60-9699-850D4D4D9FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{C850024D-092F-42CE-ADC2-874D6C29BEB8}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Item List" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Item List'!$A$1:$E$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Item List'!$A$1:$G$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="78">
   <si>
     <t>Unload timeout, retry check magazine is psnt.</t>
   </si>
@@ -190,9 +190,6 @@
     <t>Disable Map Edit</t>
   </si>
   <si>
-    <t>23/9 KN: Diable Map Edit during Auto Run.</t>
-  </si>
-  <si>
     <t>BSD015</t>
   </si>
   <si>
@@ -208,9 +205,6 @@
     <t>Error 4236 Timeout, OUT</t>
   </si>
   <si>
-    <t>Convy not move.</t>
-  </si>
-  <si>
     <t>YZ</t>
   </si>
   <si>
@@ -238,9 +232,6 @@
     <t>LYL</t>
   </si>
   <si>
-    <t>26/9 KN: ErrCode.PROGRAM_VISION_DATA_NOT_READY and Stop Program</t>
-  </si>
-  <si>
     <t>Vision Data Not Ready, machine continue to run.</t>
   </si>
   <si>
@@ -248,12 +239,51 @@
   </si>
   <si>
     <t>Out of memory DO_VISION</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Manual execute DO_HEIGHT Error Stop buzzer not mute.</t>
+  </si>
+  <si>
+    <t>Low Pressure + PusherRunConv, Manual LoadPro, Frame may flow through conveyor.</t>
+  </si>
+  <si>
+    <t>26/9 KN: 6.1.6.1 ErrCode.PROGRAM_VISION_DATA_NOT_READY and Stop Program</t>
+  </si>
+  <si>
+    <t>30/9 KN: 6.1.6.1 Update Tower Light Status</t>
+  </si>
+  <si>
+    <t>30/9 KN: 6.1.6.1 Check Low Pressure for Manual MHS Operation</t>
+  </si>
+  <si>
+    <t>23/9 KN: 6.1.6.0 Diable Map Edit during Auto Run.</t>
+  </si>
+  <si>
+    <t>BSD016</t>
+  </si>
+  <si>
+    <t>x64</t>
+  </si>
+  <si>
+    <t>6.1.5.3</t>
+  </si>
+  <si>
+    <t>Convy not move after Liifter Down. Retry not moving.</t>
+  </si>
+  <si>
+    <t>Motor Power is ON.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-14409]d\ mmmm\,\ yyyy;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -309,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -319,7 +349,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,13 +415,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>343432</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>30777</xdr:rowOff>
@@ -426,16 +459,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>297180</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>449773</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>510733</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>99106</xdr:rowOff>
+      <xdr:rowOff>541066</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -458,7 +491,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8656320" y="5052060"/>
+          <a:off x="8717280" y="5494020"/>
           <a:ext cx="2225233" cy="533446"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -788,10 +821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19A00FE7-593D-48C8-B345-574BCE73B66C}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="H13:I13"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -810,10 +843,10 @@
         <v>41</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>47</v>
@@ -933,95 +966,103 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>45561</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="2"/>
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
+        <v>74</v>
+      </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F8" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>45561</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="2"/>
+        <v>52</v>
+      </c>
+      <c r="C9" t="s">
+        <v>74</v>
+      </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F9" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>45561</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="2"/>
+        <v>51</v>
+      </c>
+      <c r="C10" t="s">
+        <v>74</v>
+      </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F10" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>45561</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="2"/>
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
+        <v>74</v>
+      </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F11" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="I11" s="2"/>
     </row>
@@ -1030,22 +1071,22 @@
         <v>45561</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="E12" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -1056,22 +1097,48 @@
       </c>
       <c r="B13" s="5"/>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="8">
+        <v>45511</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>77</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1080,298 +1147,347 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC6B51C-007F-407A-8969-4D508EF7EB4F}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="48.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="43.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="18" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="48.21875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="43.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E13" t="s">
+      <c r="G13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="D18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>36</v>
       </c>
     </row>
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6">
+        <v>45565</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6">
+        <v>45565</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E16" xr:uid="{0EC6B51C-007F-407A-8969-4D508EF7EB4F}"/>
-  <conditionalFormatting sqref="D1:D1048576">
+  <autoFilter ref="A1:G16" xr:uid="{0EC6B51C-007F-407A-8969-4D508EF7EB4F}"/>
+  <conditionalFormatting sqref="F1:F1048576">
     <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Resolution">
-      <formula>NOT(ISERROR(SEARCH("Resolution",D1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Resolution",F1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",D1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Test",F1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Monitor">
-      <formula>NOT(ISERROR(SEARCH("Monitor",D1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Monitor",F1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="Verification">
-      <formula>NOT(ISERROR(SEARCH("Verification",D1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Verification",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ver 6.1.6.3 20241026 - Release to LYL/YZ for UnisemCD - Gitted - [Request] Option_EnableProcessLog save as Setup. Default to true. Remove saving from recipe. - LYL - [Request] Set Origin clear map and run state. - LYL - [Improve] DispProg.ProgramMode, execute Yellow, Red and Buzzer, suppress Green Light to Yellow Light. - LYL
</commit_message>
<xml_diff>
--- a/Doc/UnisemCD A300 Item Tracking.xlsx
+++ b/Doc/UnisemCD A300 Item Tracking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SW_KN_2403\GitHub - Source\NDispWin5-Unisem-x64\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knboo\OneDrive - NSW Automation\Desktop\Old HDD D Drive\SW_KN_2403\GitHub - Source\NDispWin5-Unisem-x64\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245135AE-7E35-4D60-9699-850D4D4D9FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2BDF9D-08F8-4914-A629-4114C29225BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{C850024D-092F-42CE-ADC2-874D6C29BEB8}"/>
+    <workbookView xWindow="60" yWindow="60" windowWidth="28740" windowHeight="15420" activeTab="1" xr2:uid="{C850024D-092F-42CE-ADC2-874D6C29BEB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Isolated Tracking" sheetId="2" r:id="rId1"/>
@@ -19,28 +19,17 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Item List'!$A$1:$G$16</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="99">
   <si>
     <t>Unload timeout, retry check magazine is psnt.</t>
   </si>
@@ -275,6 +264,69 @@
   </si>
   <si>
     <t>Motor Power is ON.</t>
+  </si>
+  <si>
+    <t>Program Mode Tower Light Red at alarm</t>
+  </si>
+  <si>
+    <t>Process Log default enabled</t>
+  </si>
+  <si>
+    <t>Set Origin Clear Mapping and start from beginning</t>
+  </si>
+  <si>
+    <t>Log Auto Controls</t>
+  </si>
+  <si>
+    <t>26/10 KN: Log already exist in Event File since earlier time "Auto Start Run.", "Auto Stop Run.". "Change Option." was added on 6.1.5.</t>
+  </si>
+  <si>
+    <t>BSD??</t>
+  </si>
+  <si>
+    <t>Vision Fail Message. Object is currently in use elsewhere.</t>
+  </si>
+  <si>
+    <t>BSD005</t>
+  </si>
+  <si>
+    <t>Error 3999, DO_VIS_INSP Start Grab Fail</t>
+  </si>
+  <si>
+    <t>28/10 KN: High posibility camera cable connection or cable continuity.</t>
+  </si>
+  <si>
+    <t>6.1.6.2</t>
+  </si>
+  <si>
+    <t>Error 3600, Camera Comm Exception</t>
+  </si>
+  <si>
+    <t>Continuity from previous</t>
+  </si>
+  <si>
+    <t>26/10 KN: v6.1.6.3 DispProg.ProgramMode, execute Yellow, Red and Buzzer, suppress Green Light to Yellow Light.</t>
+  </si>
+  <si>
+    <t>26/10 KN: v6.1.6.3 Option_EnableProcessLog save as Setup. Default to true. Remove saving from recipe.</t>
+  </si>
+  <si>
+    <t>26/10 KN: v6.1.6.3 Set Origin Clear Run State.</t>
+  </si>
+  <si>
+    <t>RMS Download recipe name with {space} at the end. YL feedback only happen on x64 os.</t>
+  </si>
+  <si>
+    <t>Request to add log to all actions on controls</t>
+  </si>
+  <si>
+    <t>Chen</t>
+  </si>
+  <si>
+    <t>3999 Cannot load Counter Name Error, x64 on specific machine</t>
+  </si>
+  <si>
+    <t>4/11 KN: x6.1.6.3+ Encapulate EnableDebugInfo to prevent  Performance calculation when disabled.</t>
   </si>
 </sst>
 </file>
@@ -301,7 +353,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -324,22 +376,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -349,10 +390,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -821,21 +859,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19A00FE7-593D-48C8-B345-574BCE73B66C}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.88671875" customWidth="1"/>
-    <col min="7" max="7" width="30.109375" customWidth="1"/>
-    <col min="8" max="8" width="28.21875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" customWidth="1"/>
+    <col min="7" max="7" width="30.140625" customWidth="1"/>
+    <col min="8" max="8" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>46</v>
       </c>
@@ -864,7 +902,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>43</v>
       </c>
@@ -881,7 +919,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>43</v>
       </c>
@@ -898,7 +936,7 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>43</v>
       </c>
@@ -915,7 +953,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>43</v>
       </c>
@@ -932,7 +970,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>43</v>
       </c>
@@ -949,7 +987,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>43</v>
       </c>
@@ -966,7 +1004,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>45561</v>
       </c>
@@ -991,7 +1029,7 @@
       </c>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>45561</v>
       </c>
@@ -1016,7 +1054,7 @@
       </c>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>45561</v>
       </c>
@@ -1041,7 +1079,7 @@
       </c>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>45561</v>
       </c>
@@ -1066,7 +1104,7 @@
       </c>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>45561</v>
       </c>
@@ -1091,15 +1129,15 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>45560</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" t="s">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E13" s="2" t="s">
@@ -1114,20 +1152,20 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="8">
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
         <v>45511</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="2" t="s">
         <v>62</v>
       </c>
       <c r="F14" s="3" t="s">
@@ -1138,6 +1176,82 @@
       </c>
       <c r="H14" s="2" t="s">
         <v>77</v>
+      </c>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>45590</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>45592</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>45592</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1147,30 +1261,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC6B51C-007F-407A-8969-4D508EF7EB4F}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="18" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="48.21875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="43.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="48.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="43.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1187,7 +1301,7 @@
       </c>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1201,7 +1315,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1215,7 +1329,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1229,7 +1343,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1243,7 +1357,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1257,7 +1371,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1271,7 +1385,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1288,7 +1402,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1302,7 +1416,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1319,7 +1433,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1333,7 +1447,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1347,7 +1461,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1364,7 +1478,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1378,7 +1492,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1392,7 +1506,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1406,7 +1520,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1420,7 +1534,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1434,14 +1548,14 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="5">
         <v>45565</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>54</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -1454,14 +1568,14 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="5">
         <v>45565</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>54</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1472,6 +1586,131 @@
       </c>
       <c r="F20" s="1" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5">
+        <v>45582</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5">
+        <v>45582</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="5">
+        <v>45582</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5">
+        <v>45955</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="5">
+        <v>45597</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="5">
+        <v>45593</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="5">
+        <v>45600</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ver 6.1.7.1 20241209 - Remote Release to LYL/YZ/WZM for UnisemCD - Gitted - [Refactor] Removed unused frm_LotEntryOsramEMos, frm_LotEntryAnalog, frm_LotEntryAnalogPrompt, frm_LotEntryAnalogSeutp and dependencies - [Refactor] Removed unused frm_AOT_TestCloseLoop, frm_Lextart_TestCloseLoop, frm_Osram_eMos_Setup, frmDispProg_VolumeOfst and dependencies - [Improve] Added GControl.LogForm(this) the frmMVGenTLCamera - [Feature] Renamed frm_DispCore_DispSetup to frmSetupHM - [Enhance] Remove additonal space in filename for PPSelect. Suspect space from server. - [Improve] Added if (GDefineN.EnableEventDebugLog) to prevent calling Perfromance Counter methods, on possible OS corrupt system.
</commit_message>
<xml_diff>
--- a/Doc/UnisemCD A300 Item Tracking.xlsx
+++ b/Doc/UnisemCD A300 Item Tracking.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knboo\OneDrive - NSW Automation\Desktop\Old HDD D Drive\SW_KN_2403\GitHub - Source\NDispWin5-Unisem-x64\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knboo\source\repos\NSW-Software\NDispWin5-Unisem-x64\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2BDF9D-08F8-4914-A629-4114C29225BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9110590C-4214-4EB6-A631-4D4338717E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="60" windowWidth="28740" windowHeight="15420" activeTab="1" xr2:uid="{C850024D-092F-42CE-ADC2-874D6C29BEB8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C850024D-092F-42CE-ADC2-874D6C29BEB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Isolated Tracking" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="113">
   <si>
     <t>Unload timeout, retry check magazine is psnt.</t>
   </si>
@@ -327,6 +327,48 @@
   </si>
   <si>
     <t>4/11 KN: x6.1.6.3+ Encapulate EnableDebugInfo to prevent  Performance calculation when disabled.</t>
+  </si>
+  <si>
+    <t>Auto LoadPro/Return log corresponding action.</t>
+  </si>
+  <si>
+    <t>Heli Clean/Purge disable Purge Mode</t>
+  </si>
+  <si>
+    <t>Heli Pump Adj update, Ctrl 1 setting to initial settings.</t>
+  </si>
+  <si>
+    <t>Reques to add Heli Purge timer</t>
+  </si>
+  <si>
+    <t>Options&gt;Performance tab option changes add to log.</t>
+  </si>
+  <si>
+    <t>MHS&gt;Conv option change add to log.</t>
+  </si>
+  <si>
+    <t>Low Pressure setting is automatically cancel for no reason.</t>
+  </si>
+  <si>
+    <t>3/12 KN: v6.1.7.0 All control button action are logged to event.</t>
+  </si>
+  <si>
+    <t>3/12 KN: Set Ctrl Force Time Mode to false. This option for Timed mode application only.</t>
+  </si>
+  <si>
+    <t>3/12 KN: v6.1.7.0 Added Purge Timer.</t>
+  </si>
+  <si>
+    <t>3/12 KN: v6.1.7.0 Added Control Log</t>
+  </si>
+  <si>
+    <t>3/12 KN: v6.1.7.0 Removed Cancel Button</t>
+  </si>
+  <si>
+    <t>3/12 KN: Use PumpAdj, parameter for PumpAdj is priotiy</t>
+  </si>
+  <si>
+    <t>8/12 KN: v6.1.7.0 Trim spaces.</t>
   </si>
 </sst>
 </file>
@@ -380,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -391,6 +433,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,6 +576,138 @@
         <a:xfrm>
           <a:off x="8717280" y="5494020"/>
           <a:ext cx="2225233" cy="533446"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>552859</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>581098</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C63B7F4-7D7C-3DF0-3AAD-1CA4E4D51A84}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10115550" y="12115800"/>
+          <a:ext cx="2934109" cy="523948"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19048</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>40584</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>557016</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>163286</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40CF6A91-918A-1DFC-7C27-E7659AF26331}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10265227" y="10763013"/>
+          <a:ext cx="9722789" cy="1401773"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>17095</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>183502</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75AEFD36-0D41-0464-9333-EAE6C4573094}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13693588" y="12057529"/>
+          <a:ext cx="6068272" cy="6077798"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1261,16 +1438,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC6B51C-007F-407A-8969-4D508EF7EB4F}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="18" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.140625" style="5" customWidth="1"/>
     <col min="4" max="4" width="48.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="43.28515625" style="1" customWidth="1"/>
@@ -1681,8 +1858,11 @@
       <c r="D25" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E25" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1694,6 +1874,9 @@
       </c>
       <c r="D26" s="1" t="s">
         <v>95</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1711,6 +1894,125 @@
       </c>
       <c r="E27" s="1" t="s">
         <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="5">
+        <v>45625</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="5">
+        <v>45625</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="5">
+        <v>45625</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="5">
+        <v>45625</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="5">
+        <v>45625</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="5">
+        <v>45625</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="5">
+        <v>45625</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>